<commit_message>
PROS-8674 MARSIN_SAND template correct
</commit_message>
<xml_diff>
--- a/Projects/MARSIN_SAND/Data/Template.xlsx
+++ b/Projects/MARSIN_SAND/Data/Template.xlsx
@@ -44,6 +44,8 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Product Group Adjacency'!$A$2:$T$8</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Product Group Adjacency'!$A$2:$T$8</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Product Group Adjacency'!$A$2:$T$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Product Group Adjacency'!$A$2:$T$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Product Group Adjacency'!$A$2:$T$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2521" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2521" uniqueCount="155">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -337,9 +339,6 @@
   </si>
   <si>
     <t xml:space="preserve">8410136004018 / 18853301550045, 8410136004056, 8410136004117 / 18853301550021, 8410136004193, 8410136004155, 8410136004094, 8410136004070, 8410136004179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N / A</t>
   </si>
   <si>
     <t xml:space="preserve">8410136004018 / 18853301550045, 8410136004056, 8410136004117 / 18853301550021, 8410136004193, 8410136004155, 8410136004094, 8410136004179</t>
@@ -1259,19 +1258,19 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F28" activeCellId="3" sqref="E31:E36 E38 E40 F28"/>
+      <selection pane="bottomLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="1016" min="10" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.57085020242915"/>
   </cols>
@@ -36214,17 +36213,17 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31:E36 E38 E40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="31.9230769230769"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.57085020242915"/>
@@ -36232,7 +36231,7 @@
     <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="17" min="16" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="20" min="19" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.57085020242915"/>
   </cols>
@@ -38684,7 +38683,7 @@
         <v>93</v>
       </c>
       <c r="F42" s="26" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="G42" s="26" t="s">
         <v>55</v>
@@ -38741,7 +38740,7 @@
         <v>52</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F43" s="26" t="s">
         <v>55</v>
@@ -38801,7 +38800,7 @@
         <v>52</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F44" s="25" t="s">
         <v>55</v>
@@ -38861,7 +38860,7 @@
         <v>52</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F45" s="25" t="s">
         <v>55</v>
@@ -38921,7 +38920,7 @@
         <v>52</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F46" s="25" t="s">
         <v>55</v>
@@ -38981,7 +38980,7 @@
         <v>52</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F47" s="25" t="s">
         <v>55</v>
@@ -39041,7 +39040,7 @@
         <v>52</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F48" s="25" t="s">
         <v>55</v>
@@ -39101,7 +39100,7 @@
         <v>52</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F49" s="25" t="s">
         <v>55</v>
@@ -39160,10 +39159,10 @@
         <v>2</v>
       </c>
       <c r="D50" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="22" t="s">
         <v>102</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>103</v>
       </c>
       <c r="F50" s="34" t="n">
         <v>4</v>
@@ -39346,10 +39345,10 @@
         <v>2</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F53" s="34" t="s">
         <v>55</v>
@@ -39408,10 +39407,10 @@
         <v>1</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F54" s="34" t="s">
         <v>55</v>
@@ -39532,10 +39531,10 @@
         <v>2</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F56" s="34" t="s">
         <v>55</v>
@@ -39656,10 +39655,10 @@
         <v>2</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F58" s="34" t="s">
         <v>55</v>
@@ -39718,10 +39717,10 @@
         <v>1</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F59" s="34" t="s">
         <v>55</v>
@@ -39842,10 +39841,10 @@
         <v>3</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F61" s="34" t="s">
         <v>55</v>
@@ -39902,10 +39901,10 @@
       </c>
       <c r="C62" s="22"/>
       <c r="D62" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E62" s="37" t="s">
         <v>109</v>
-      </c>
-      <c r="E62" s="37" t="s">
-        <v>110</v>
       </c>
       <c r="F62" s="34" t="s">
         <v>55</v>
@@ -40024,10 +40023,10 @@
       </c>
       <c r="C64" s="22"/>
       <c r="D64" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F64" s="34" t="s">
         <v>55</v>
@@ -40089,7 +40088,7 @@
         <v>29</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F65" s="26" t="s">
         <v>55</v>
@@ -40147,10 +40146,10 @@
       </c>
       <c r="C66" s="22"/>
       <c r="D66" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F66" s="34" t="s">
         <v>55</v>
@@ -40269,10 +40268,10 @@
       </c>
       <c r="C68" s="22"/>
       <c r="D68" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F68" s="39" t="n">
         <v>1</v>
@@ -40455,10 +40454,10 @@
         <v>3</v>
       </c>
       <c r="D71" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F71" s="39" t="s">
         <v>55</v>
@@ -40579,10 +40578,10 @@
         <v>4</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E73" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F73" s="39" t="s">
         <v>55</v>
@@ -40668,15 +40667,15 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N5" activeCellId="3" sqref="E31:E36 E38 E40 N5"/>
+      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3481781376518"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.49797570850202"/>
@@ -40740,10 +40739,10 @@
         <v>46</v>
       </c>
       <c r="D2" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="42" t="s">
         <v>115</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>116</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>48</v>
@@ -40796,10 +40795,10 @@
         <v>52</v>
       </c>
       <c r="D3" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="45" t="s">
         <v>117</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>118</v>
       </c>
       <c r="F3" s="39" t="s">
         <v>54</v>
@@ -40920,10 +40919,10 @@
         <v>52</v>
       </c>
       <c r="D5" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="45" t="s">
         <v>119</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>120</v>
       </c>
       <c r="F5" s="39" t="s">
         <v>54</v>
@@ -41044,10 +41043,10 @@
         <v>52</v>
       </c>
       <c r="D7" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="45" t="s">
         <v>121</v>
-      </c>
-      <c r="E7" s="45" t="s">
-        <v>122</v>
       </c>
       <c r="F7" s="39" t="s">
         <v>54</v>
@@ -41106,10 +41105,10 @@
         <v>52</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F8" s="39" t="s">
         <v>56</v>
@@ -41185,17 +41184,17 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V10" activeCellId="3" sqref="E31:E36 E38 E40 V10"/>
+      <selection pane="topLeft" activeCell="V10" activeCellId="0" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.8785425101215"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -41244,16 +41243,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="E2" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="F2" s="42" t="s">
         <v>126</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>127</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>48</v>
@@ -41309,10 +41308,10 @@
         <v>31</v>
       </c>
       <c r="E3" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="22" t="s">
         <v>128</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>129</v>
       </c>
       <c r="G3" s="39" t="s">
         <v>55</v>
@@ -41374,10 +41373,10 @@
         <v>31</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>55</v>
@@ -41500,10 +41499,10 @@
         <v>33</v>
       </c>
       <c r="E6" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="57" t="s">
         <v>128</v>
-      </c>
-      <c r="F6" s="57" t="s">
-        <v>129</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>55</v>
@@ -41565,10 +41564,10 @@
         <v>33</v>
       </c>
       <c r="E7" s="57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7" s="54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>55</v>
@@ -41703,15 +41702,15 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="3" sqref="E31:E36 E38 E40 T2"/>
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.0566801619433"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.2348178137652"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="17" min="6" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="19" min="18" style="0" width="13.3886639676113"/>
@@ -41763,13 +41762,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="E2" s="42" t="s">
         <v>132</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>133</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>48</v>
@@ -41822,10 +41821,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" s="62" t="s">
         <v>134</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>135</v>
       </c>
       <c r="F3" s="63" t="s">
         <v>54</v>
@@ -41884,10 +41883,10 @@
         <v>6</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F4" s="64" t="s">
         <v>55</v>
@@ -41946,10 +41945,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F5" s="64" t="s">
         <v>55</v>
@@ -42008,10 +42007,10 @@
         <v>12</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F6" s="64" t="s">
         <v>55</v>
@@ -42070,10 +42069,10 @@
         <v>15</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F7" s="64" t="s">
         <v>55</v>
@@ -42132,10 +42131,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="62" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F8" s="63" t="s">
         <v>54</v>
@@ -42194,10 +42193,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F9" s="64" t="s">
         <v>55</v>
@@ -42256,10 +42255,10 @@
         <v>10</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E10" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F10" s="64" t="s">
         <v>55</v>
@@ -42318,10 +42317,10 @@
         <v>13</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F11" s="64" t="s">
         <v>55</v>
@@ -42380,10 +42379,10 @@
         <v>16</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F12" s="64" t="s">
         <v>55</v>
@@ -42442,10 +42441,10 @@
         <v>3</v>
       </c>
       <c r="D13" s="62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E13" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F13" s="63" t="s">
         <v>54</v>
@@ -42504,10 +42503,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E14" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14" s="63" t="s">
         <v>54</v>
@@ -42566,10 +42565,10 @@
         <v>5</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F15" s="63" t="s">
         <v>54</v>
@@ -42628,10 +42627,10 @@
         <v>8</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E16" s="65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F16" s="64" t="s">
         <v>55</v>
@@ -42690,10 +42689,10 @@
         <v>11</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F17" s="64" t="s">
         <v>55</v>
@@ -42752,10 +42751,10 @@
         <v>14</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F18" s="64" t="s">
         <v>55</v>
@@ -42814,10 +42813,10 @@
         <v>17</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E19" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F19" s="64" t="s">
         <v>55</v>
@@ -42891,20 +42890,20 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="3" sqref="E31:E36 E38 E40 T2"/>
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.8502024291498"/>
     <col collapsed="false" hidden="false" max="17" min="6" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -42955,10 +42954,10 @@
         <v>46</v>
       </c>
       <c r="D2" s="71" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="71" t="s">
         <v>143</v>
-      </c>
-      <c r="E2" s="71" t="s">
-        <v>144</v>
       </c>
       <c r="F2" s="68" t="s">
         <v>48</v>
@@ -43014,7 +43013,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F3" s="74" t="n">
         <v>0.55</v>
@@ -43076,7 +43075,7 @@
         <v>31</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F4" s="75" t="s">
         <v>55</v>
@@ -43138,7 +43137,7 @@
         <v>30</v>
       </c>
       <c r="E5" s="78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F5" s="74" t="n">
         <v>0.75</v>
@@ -43200,7 +43199,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F6" s="75" t="s">
         <v>55</v>
@@ -43262,7 +43261,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" s="75" t="s">
         <v>55</v>
@@ -43321,10 +43320,10 @@
         <v>29</v>
       </c>
       <c r="D8" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="52" t="s">
         <v>150</v>
-      </c>
-      <c r="E8" s="52" t="s">
-        <v>151</v>
       </c>
       <c r="F8" s="79" t="n">
         <v>0.3</v>
@@ -43386,7 +43385,7 @@
         <v>33</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F9" s="79" t="n">
         <v>0.6</v>
@@ -43448,7 +43447,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F10" s="75" t="s">
         <v>55</v>
@@ -43510,7 +43509,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F11" s="79" t="n">
         <v>0.8</v>
@@ -43572,7 +43571,7 @@
         <v>34</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F12" s="75" t="s">
         <v>55</v>
@@ -43645,19 +43644,19 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="2" sqref="E31:E36 E38 E40"/>
+      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
PROS-10319-Update Template for biscrok spelling
</commit_message>
<xml_diff>
--- a/Projects/MARSIN_SAND/Data/Template.xlsx
+++ b/Projects/MARSIN_SAND/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,6 +46,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Product Group Adjacency'!$A$2:$T$8</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Product Group Adjacency'!$A$2:$T$8</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Product Group Adjacency'!$A$2:$T$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Product Group Adjacency'!$A$2:$T$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -447,7 +448,7 @@
     <t xml:space="preserve">18906002483171, 18906002489043, 8906002480203, 18906002483188, 18906002481436</t>
   </si>
   <si>
-    <t xml:space="preserve">Biscrock : Care &amp; Treat</t>
+    <t xml:space="preserve">Biscrok : Care &amp; Treat</t>
   </si>
   <si>
     <t xml:space="preserve">Block Entity</t>
@@ -1263,22 +1264,22 @@
   </sheetPr>
   <dimension ref="1:45"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="99" zoomScaleNormal="99" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="99" zoomScaleNormal="99" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.8866396761134"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="35.8866396761134"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="1016" min="10" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1017" style="0" width="8.57085020242915"/>
   </cols>
@@ -36321,17 +36322,17 @@
   </sheetPr>
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E78" activeCellId="0" sqref="E78"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E50" activeCellId="0" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="74.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="75.6275303643725"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.57085020242915"/>
@@ -36339,7 +36340,7 @@
     <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="17" min="16" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="20" min="19" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.57085020242915"/>
   </cols>
@@ -41064,15 +41065,15 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.2064777327935"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.49797570850202"/>
@@ -41553,7 +41554,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="48" t="s">
         <v>17</v>
       </c>
@@ -41648,12 +41649,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.4858299595142"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -42166,10 +42167,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.412955465587"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.0566801619433"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="17" min="6" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="19" min="18" style="0" width="13.3886639676113"/>
@@ -43540,15 +43541,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.919028340081"/>
     <col collapsed="false" hidden="false" max="17" min="6" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -44288,20 +44289,20 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>